<commit_message>
Refs #5722.  Refs #5723.
Column re-alignment corrections.
</commit_message>
<xml_diff>
--- a/spec/test_data/conversion_employees/sample_conversion_employees.xlsx
+++ b/spec/test_data/conversion_employees/sample_conversion_employees.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="174">
   <si>
     <t>Action</t>
   </si>
@@ -538,6 +538,9 @@
   </si>
   <si>
     <t>Daughter</t>
+  </si>
+  <si>
+    <t>Hire Date</t>
   </si>
 </sst>
 </file>
@@ -907,13 +910,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:EU2"/>
+  <dimension ref="A1:EV2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:151">
+    <row r="1" spans="1:152">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -936,439 +941,442 @@
         <v>6</v>
       </c>
       <c r="H1" t="s">
+        <v>173</v>
+      </c>
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AL1" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AM1" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AN1" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AO1" t="s">
         <v>39</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AP1" t="s">
         <v>40</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AQ1" t="s">
         <v>41</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AR1" t="s">
         <v>42</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AS1" t="s">
         <v>43</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AT1" t="s">
         <v>44</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AU1" t="s">
         <v>45</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="AV1" t="s">
         <v>46</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="AW1" t="s">
         <v>47</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="AX1" t="s">
         <v>48</v>
       </c>
-      <c r="AX1" t="s">
+      <c r="AY1" t="s">
         <v>49</v>
       </c>
-      <c r="AY1" t="s">
+      <c r="AZ1" t="s">
         <v>50</v>
       </c>
-      <c r="AZ1" t="s">
+      <c r="BA1" t="s">
         <v>51</v>
       </c>
-      <c r="BA1" t="s">
+      <c r="BB1" t="s">
         <v>52</v>
       </c>
-      <c r="BB1" t="s">
+      <c r="BC1" t="s">
         <v>53</v>
       </c>
-      <c r="BC1" t="s">
+      <c r="BD1" t="s">
         <v>54</v>
       </c>
-      <c r="BD1" t="s">
+      <c r="BE1" t="s">
         <v>55</v>
       </c>
-      <c r="BE1" t="s">
+      <c r="BF1" t="s">
         <v>56</v>
       </c>
-      <c r="BF1" t="s">
+      <c r="BG1" t="s">
         <v>57</v>
       </c>
-      <c r="BG1" t="s">
+      <c r="BH1" t="s">
         <v>58</v>
       </c>
-      <c r="BH1" t="s">
+      <c r="BI1" t="s">
         <v>59</v>
       </c>
-      <c r="BI1" t="s">
+      <c r="BJ1" t="s">
         <v>60</v>
       </c>
-      <c r="BJ1" t="s">
+      <c r="BK1" t="s">
         <v>61</v>
       </c>
-      <c r="BK1" t="s">
+      <c r="BL1" t="s">
         <v>62</v>
       </c>
-      <c r="BL1" t="s">
+      <c r="BM1" t="s">
         <v>63</v>
       </c>
-      <c r="BM1" t="s">
+      <c r="BN1" t="s">
         <v>64</v>
       </c>
-      <c r="BN1" t="s">
+      <c r="BO1" t="s">
         <v>65</v>
       </c>
-      <c r="BO1" t="s">
+      <c r="BP1" t="s">
         <v>66</v>
       </c>
-      <c r="BP1" t="s">
+      <c r="BQ1" t="s">
         <v>67</v>
       </c>
-      <c r="BQ1" t="s">
+      <c r="BR1" t="s">
         <v>68</v>
       </c>
-      <c r="BR1" t="s">
+      <c r="BS1" t="s">
         <v>69</v>
       </c>
-      <c r="BS1" t="s">
+      <c r="BT1" t="s">
         <v>70</v>
       </c>
-      <c r="BT1" t="s">
+      <c r="BU1" t="s">
         <v>71</v>
       </c>
-      <c r="BU1" t="s">
+      <c r="BV1" t="s">
         <v>72</v>
       </c>
-      <c r="BV1" t="s">
+      <c r="BW1" t="s">
         <v>73</v>
       </c>
-      <c r="BW1" t="s">
+      <c r="BX1" t="s">
         <v>74</v>
       </c>
-      <c r="BX1" t="s">
+      <c r="BY1" t="s">
         <v>75</v>
       </c>
-      <c r="BY1" t="s">
+      <c r="BZ1" t="s">
         <v>76</v>
       </c>
-      <c r="BZ1" t="s">
+      <c r="CA1" t="s">
         <v>77</v>
       </c>
-      <c r="CA1" t="s">
+      <c r="CB1" t="s">
         <v>78</v>
       </c>
-      <c r="CB1" t="s">
+      <c r="CC1" t="s">
         <v>79</v>
       </c>
-      <c r="CC1" t="s">
+      <c r="CD1" t="s">
         <v>80</v>
       </c>
-      <c r="CD1" t="s">
+      <c r="CE1" t="s">
         <v>81</v>
       </c>
-      <c r="CE1" t="s">
+      <c r="CF1" t="s">
         <v>82</v>
       </c>
-      <c r="CF1" t="s">
+      <c r="CG1" t="s">
         <v>83</v>
       </c>
-      <c r="CG1" t="s">
+      <c r="CH1" t="s">
         <v>84</v>
       </c>
-      <c r="CH1" t="s">
+      <c r="CI1" t="s">
         <v>85</v>
       </c>
-      <c r="CI1" t="s">
+      <c r="CJ1" t="s">
         <v>86</v>
       </c>
-      <c r="CJ1" t="s">
+      <c r="CK1" t="s">
         <v>87</v>
       </c>
-      <c r="CK1" t="s">
+      <c r="CL1" t="s">
         <v>88</v>
       </c>
-      <c r="CL1" t="s">
+      <c r="CM1" t="s">
         <v>89</v>
       </c>
-      <c r="CM1" t="s">
+      <c r="CN1" t="s">
         <v>90</v>
       </c>
-      <c r="CN1" t="s">
+      <c r="CO1" t="s">
         <v>91</v>
       </c>
-      <c r="CO1" t="s">
+      <c r="CP1" t="s">
         <v>92</v>
       </c>
-      <c r="CP1" t="s">
+      <c r="CQ1" t="s">
         <v>93</v>
       </c>
-      <c r="CQ1" t="s">
+      <c r="CR1" t="s">
         <v>94</v>
       </c>
-      <c r="CR1" t="s">
+      <c r="CS1" t="s">
         <v>95</v>
       </c>
-      <c r="CS1" t="s">
+      <c r="CT1" t="s">
         <v>96</v>
       </c>
-      <c r="CT1" t="s">
+      <c r="CU1" t="s">
         <v>97</v>
       </c>
-      <c r="CU1" t="s">
+      <c r="CV1" t="s">
         <v>98</v>
       </c>
-      <c r="CV1" t="s">
+      <c r="CW1" t="s">
         <v>99</v>
       </c>
-      <c r="CW1" t="s">
+      <c r="CX1" t="s">
         <v>100</v>
       </c>
-      <c r="CX1" t="s">
+      <c r="CY1" t="s">
         <v>101</v>
       </c>
-      <c r="CY1" t="s">
+      <c r="CZ1" t="s">
         <v>102</v>
       </c>
-      <c r="CZ1" t="s">
+      <c r="DA1" t="s">
         <v>103</v>
       </c>
-      <c r="DA1" t="s">
+      <c r="DB1" t="s">
         <v>104</v>
       </c>
-      <c r="DB1" t="s">
+      <c r="DC1" t="s">
         <v>105</v>
       </c>
-      <c r="DC1" t="s">
+      <c r="DD1" t="s">
         <v>106</v>
       </c>
-      <c r="DD1" t="s">
+      <c r="DE1" t="s">
         <v>107</v>
       </c>
-      <c r="DE1" t="s">
+      <c r="DF1" t="s">
         <v>108</v>
       </c>
-      <c r="DF1" t="s">
+      <c r="DG1" t="s">
         <v>109</v>
       </c>
-      <c r="DG1" t="s">
+      <c r="DH1" t="s">
         <v>110</v>
       </c>
-      <c r="DH1" t="s">
+      <c r="DI1" t="s">
         <v>111</v>
       </c>
-      <c r="DI1" t="s">
+      <c r="DJ1" t="s">
         <v>112</v>
       </c>
-      <c r="DJ1" t="s">
+      <c r="DK1" t="s">
         <v>113</v>
       </c>
-      <c r="DK1" t="s">
+      <c r="DL1" t="s">
         <v>114</v>
       </c>
-      <c r="DL1" t="s">
+      <c r="DM1" t="s">
         <v>115</v>
       </c>
-      <c r="DM1" t="s">
+      <c r="DN1" t="s">
         <v>116</v>
       </c>
-      <c r="DN1" t="s">
+      <c r="DO1" t="s">
         <v>117</v>
       </c>
-      <c r="DO1" t="s">
+      <c r="DP1" t="s">
         <v>118</v>
       </c>
-      <c r="DP1" t="s">
+      <c r="DQ1" t="s">
         <v>119</v>
       </c>
-      <c r="DQ1" t="s">
+      <c r="DR1" t="s">
         <v>120</v>
       </c>
-      <c r="DR1" t="s">
+      <c r="DS1" t="s">
         <v>121</v>
       </c>
-      <c r="DS1" t="s">
+      <c r="DT1" t="s">
         <v>122</v>
       </c>
-      <c r="DT1" t="s">
+      <c r="DU1" t="s">
         <v>123</v>
       </c>
-      <c r="DU1" t="s">
+      <c r="DV1" t="s">
         <v>124</v>
       </c>
-      <c r="DV1" t="s">
+      <c r="DW1" t="s">
         <v>125</v>
       </c>
-      <c r="DW1" t="s">
+      <c r="DX1" t="s">
         <v>126</v>
       </c>
-      <c r="DX1" t="s">
+      <c r="DY1" t="s">
         <v>127</v>
       </c>
-      <c r="DY1" t="s">
+      <c r="DZ1" t="s">
         <v>128</v>
       </c>
-      <c r="DZ1" t="s">
+      <c r="EA1" t="s">
         <v>129</v>
       </c>
-      <c r="EA1" t="s">
+      <c r="EB1" t="s">
         <v>130</v>
       </c>
-      <c r="EB1" t="s">
+      <c r="EC1" t="s">
         <v>131</v>
       </c>
-      <c r="EC1" t="s">
+      <c r="ED1" t="s">
         <v>132</v>
       </c>
-      <c r="ED1" t="s">
+      <c r="EE1" t="s">
         <v>133</v>
       </c>
-      <c r="EE1" t="s">
+      <c r="EF1" t="s">
         <v>134</v>
       </c>
-      <c r="EF1" t="s">
+      <c r="EG1" t="s">
         <v>135</v>
       </c>
-      <c r="EG1" t="s">
+      <c r="EH1" t="s">
         <v>136</v>
       </c>
-      <c r="EH1" t="s">
+      <c r="EI1" t="s">
         <v>137</v>
       </c>
-      <c r="EI1" t="s">
+      <c r="EJ1" t="s">
         <v>138</v>
       </c>
-      <c r="EJ1" t="s">
+      <c r="EK1" t="s">
         <v>139</v>
       </c>
-      <c r="EK1" t="s">
+      <c r="EL1" t="s">
         <v>140</v>
       </c>
-      <c r="EL1" t="s">
+      <c r="EM1" t="s">
         <v>141</v>
       </c>
-      <c r="EM1" t="s">
+      <c r="EN1" t="s">
         <v>142</v>
       </c>
-      <c r="EN1" t="s">
+      <c r="EO1" t="s">
         <v>143</v>
       </c>
-      <c r="EO1" t="s">
+      <c r="EP1" t="s">
         <v>144</v>
       </c>
-      <c r="EP1" t="s">
+      <c r="EQ1" t="s">
         <v>145</v>
       </c>
-      <c r="EQ1" t="s">
+      <c r="ER1" t="s">
         <v>146</v>
       </c>
-      <c r="ER1" t="s">
+      <c r="ES1" t="s">
         <v>147</v>
       </c>
-      <c r="ES1" t="s">
+      <c r="ET1" t="s">
         <v>148</v>
       </c>
-      <c r="ET1" t="s">
+      <c r="EU1" t="s">
         <v>149</v>
       </c>
-      <c r="EU1" t="s">
+      <c r="EV1" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="2" spans="1:151">
+    <row r="2" spans="1:152">
       <c r="A2" t="s">
         <v>151</v>
       </c>
@@ -1384,106 +1392,106 @@
       <c r="E2">
         <v>202187000</v>
       </c>
-      <c r="H2" s="1">
+      <c r="I2" s="1">
         <v>40724</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>155</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>156</v>
       </c>
-      <c r="N2">
+      <c r="O2">
         <v>830.75</v>
       </c>
-      <c r="Q2">
+      <c r="R2">
         <v>219000368</v>
       </c>
-      <c r="R2" s="1">
+      <c r="S2" s="1">
         <v>21349</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
         <v>157</v>
       </c>
-      <c r="T2">
+      <c r="U2">
         <v>344.57</v>
       </c>
-      <c r="U2" t="s">
+      <c r="V2" t="s">
         <v>158</v>
       </c>
-      <c r="V2" t="s">
+      <c r="W2" t="s">
         <v>159</v>
       </c>
-      <c r="W2" t="s">
+      <c r="X2" t="s">
         <v>160</v>
-      </c>
-      <c r="X2" t="s">
-        <v>161</v>
       </c>
       <c r="Y2" t="s">
         <v>161</v>
       </c>
       <c r="Z2" t="s">
+        <v>161</v>
+      </c>
+      <c r="AA2" t="s">
         <v>162</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AB2" t="s">
         <v>161</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AC2" t="s">
         <v>163</v>
       </c>
-      <c r="AC2" t="s">
+      <c r="AD2" t="s">
         <v>164</v>
       </c>
-      <c r="AD2">
+      <c r="AE2">
         <v>20737</v>
       </c>
-      <c r="AE2" t="s">
+      <c r="AF2" t="s">
         <v>165</v>
       </c>
-      <c r="AF2">
+      <c r="AG2">
         <v>213000000</v>
       </c>
-      <c r="AG2" s="1">
+      <c r="AH2" s="1">
         <v>38565</v>
       </c>
-      <c r="AH2" t="s">
+      <c r="AI2" t="s">
         <v>166</v>
       </c>
-      <c r="AI2">
+      <c r="AJ2">
         <v>486.18</v>
       </c>
-      <c r="AJ2" t="s">
+      <c r="AK2" t="s">
         <v>158</v>
       </c>
-      <c r="AK2" t="s">
+      <c r="AL2" t="s">
         <v>167</v>
       </c>
-      <c r="AL2" t="s">
+      <c r="AM2" t="s">
         <v>168</v>
       </c>
-      <c r="AT2" t="s">
+      <c r="AU2" t="s">
         <v>169</v>
       </c>
-      <c r="AU2" t="s">
+      <c r="AV2" t="s">
         <v>161</v>
       </c>
-      <c r="AV2" s="1">
+      <c r="AW2" s="1">
         <v>39154</v>
       </c>
-      <c r="AW2" t="s">
+      <c r="AX2" t="s">
         <v>157</v>
       </c>
-      <c r="AY2" t="s">
+      <c r="AZ2" t="s">
         <v>170</v>
       </c>
-      <c r="AZ2" t="s">
+      <c r="BA2" t="s">
         <v>171</v>
       </c>
-      <c r="BA2" t="s">
+      <c r="BB2" t="s">
         <v>172</v>
       </c>
-      <c r="BI2" t="s">
+      <c r="BJ2" t="s">
         <v>169</v>
       </c>
     </row>

</xml_diff>